<commit_message>
updated with accurate data for scaling
</commit_message>
<xml_diff>
--- a/data/Data_Test2.xlsx
+++ b/data/Data_Test2.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tatianakalainoff/Documents/GitHub/major-studio-2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7799ECF3-C0B8-8C43-ADDA-1DF68ABC9D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D6CB4F-7FD6-3C40-A99F-DA6ED29E88E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="920" windowWidth="27640" windowHeight="15680" xr2:uid="{067C5572-058F-1F42-B9D0-4CDC9E502D42}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$91</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,9 +47,6 @@
     <t>radiusTop</t>
   </si>
   <si>
-    <t>radiusBottom</t>
-  </si>
-  <si>
     <t>color</t>
   </si>
   <si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>white</t>
+  </si>
+  <si>
+    <t>OG DATA</t>
   </si>
 </sst>
 </file>
@@ -416,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4328A730-E7CA-3945-A5F9-D48A384393CA}">
   <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="I82" sqref="I82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -433,426 +436,442 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2022</v>
+        <v>1993</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2022</v>
+        <v>1993</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3">
-        <v>12</v>
+        <f>SUM(C2,D3)</f>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>2022</v>
+        <v>1993</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <f>SUM(C3,D4)</f>
+        <v>10</v>
+      </c>
+      <c r="D4">
         <v>9</v>
       </c>
-      <c r="C4">
-        <v>45</v>
-      </c>
-      <c r="D4">
-        <v>45</v>
-      </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>2021</v>
+        <v>1994</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2021</v>
+        <v>1994</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6">
-        <v>20</v>
+        <f>SUM(C5,D6)</f>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2021</v>
+        <v>1994</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7">
-        <v>30</v>
+        <f>SUM(C6,D7)</f>
+        <v>5</v>
       </c>
       <c r="D7">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>2020</v>
+        <v>1995</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>2020</v>
+        <v>1995</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9">
-        <v>22</v>
+        <f>SUM(C8,D9)</f>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>2020</v>
+        <v>1995</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10">
-        <v>37</v>
+        <f>SUM(C9,D10)</f>
+        <v>10</v>
       </c>
       <c r="D10">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>2019</v>
+        <v>1996</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>2019</v>
+        <v>1996</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12">
-        <v>16</v>
+        <f>SUM(C11,D12)</f>
+        <v>2</v>
       </c>
       <c r="D12">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>2019</v>
+        <v>1996</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13">
-        <v>39</v>
+        <f>SUM(C12,D13)</f>
+        <v>10</v>
       </c>
       <c r="D13">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>2018</v>
+        <v>1997</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>2018</v>
+        <v>1997</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15">
-        <v>16</v>
+        <f>SUM(C14,D15)</f>
+        <v>2</v>
       </c>
       <c r="D15">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>2018</v>
+        <v>1997</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16">
-        <v>37</v>
+        <f>SUM(C15,D16)</f>
+        <v>15</v>
       </c>
       <c r="D16">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>2017</v>
+        <v>1998</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>2017</v>
+        <v>1998</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18">
-        <v>10</v>
+        <f>SUM(C17,D18)</f>
+        <v>2</v>
       </c>
       <c r="D18">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>2017</v>
+        <v>1998</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C19">
-        <v>46</v>
+        <f>SUM(C18,D19)</f>
+        <v>10</v>
       </c>
       <c r="D19">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>2016</v>
+        <v>1999</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>2016</v>
+        <v>1999</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21">
-        <v>13</v>
+        <f>SUM(C20,D21)</f>
+        <v>2</v>
       </c>
       <c r="D21">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>2016</v>
+        <v>1999</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>40</v>
+        <f>SUM(C21,D22)</f>
+        <v>16</v>
       </c>
       <c r="D22">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="E22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>2015</v>
+        <v>2000</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>2015</v>
+        <v>2000</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24">
-        <v>14</v>
+        <f>SUM(C23,D24)</f>
+        <v>3</v>
       </c>
       <c r="D24">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>2015</v>
+        <v>2000</v>
       </c>
       <c r="B25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C25">
-        <v>41</v>
+        <f>SUM(C24,D25)</f>
+        <v>10</v>
       </c>
       <c r="D25">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>2014</v>
+        <v>2001</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -861,661 +880,687 @@
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>2014</v>
+        <v>2001</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27">
-        <v>15</v>
+        <f>SUM(C26,D27)</f>
+        <v>2</v>
       </c>
       <c r="D27">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>2014</v>
+        <v>2001</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C28">
-        <v>45</v>
+        <f>SUM(C27,D28)</f>
+        <v>17</v>
       </c>
       <c r="D28">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="E28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>2013</v>
+        <v>2002</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D29">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>2013</v>
+        <v>2002</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <f>SUM(C29,D30)</f>
+        <v>2</v>
       </c>
       <c r="D30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>2013</v>
+        <v>2002</v>
       </c>
       <c r="B31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C31">
-        <v>41</v>
+        <f>SUM(C30,D31)</f>
+        <v>13</v>
       </c>
       <c r="D31">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="E31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>2012</v>
+        <v>2003</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>2012</v>
+        <v>2003</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C33">
-        <v>10</v>
+        <f>SUM(C32,D33)</f>
+        <v>4</v>
       </c>
       <c r="D33">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>2012</v>
+        <v>2003</v>
       </c>
       <c r="B34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C34">
-        <v>28</v>
+        <f>SUM(C33,D34)</f>
+        <v>24</v>
       </c>
       <c r="D34">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>2011</v>
+        <v>2004</v>
       </c>
       <c r="B35" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>2011</v>
+        <v>2004</v>
       </c>
       <c r="B36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C36">
-        <v>7</v>
+        <f>SUM(C35,D36)</f>
+        <v>6</v>
       </c>
       <c r="D36">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>2011</v>
+        <v>2004</v>
       </c>
       <c r="B37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C37">
-        <v>44</v>
+        <f>SUM(C36,D37)</f>
+        <v>23</v>
       </c>
       <c r="D37">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="E37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>2010</v>
+        <v>2005</v>
       </c>
       <c r="B38" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>2010</v>
+        <v>2005</v>
       </c>
       <c r="B39" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C39">
+        <f>SUM(C38,D39)</f>
         <v>3</v>
       </c>
       <c r="D39">
         <v>3</v>
       </c>
       <c r="E39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>2010</v>
+        <v>2005</v>
       </c>
       <c r="B40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C40">
-        <v>27</v>
+        <f>SUM(C39,D40)</f>
+        <v>24</v>
       </c>
       <c r="D40">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>2009</v>
+        <v>2006</v>
       </c>
       <c r="B41" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E41" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>2009</v>
+        <v>2006</v>
       </c>
       <c r="B42" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C42">
-        <v>5</v>
+        <f>SUM(C41,D42)</f>
+        <v>4</v>
       </c>
       <c r="D42">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>2009</v>
+        <v>2006</v>
       </c>
       <c r="B43" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C43">
-        <v>31</v>
+        <f>SUM(C42,D43)</f>
+        <v>21</v>
       </c>
       <c r="D43">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E43" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="B44" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E44" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="B45" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <f>SUM(C44,D45)</f>
+        <v>5</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E45" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="B46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C46">
-        <v>17</v>
+        <f>SUM(C45,D46)</f>
+        <v>25</v>
       </c>
       <c r="D46">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="B47" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C47">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D47">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E47" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="B48" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C48">
-        <v>3</v>
+        <f>SUM(C47,D48)</f>
+        <v>1</v>
       </c>
       <c r="D48">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="B49" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C49">
-        <v>20</v>
+        <f>SUM(C48,D49)</f>
+        <v>18</v>
       </c>
       <c r="D49">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E49" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="B50" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="B51" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C51">
-        <v>4</v>
+        <f>SUM(C50,D51)</f>
+        <v>6</v>
       </c>
       <c r="D51">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E51" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="B52" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C52">
-        <v>17</v>
+        <f>SUM(C51,D52)</f>
+        <v>37</v>
       </c>
       <c r="D52">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E52" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>2005</v>
+        <v>2010</v>
       </c>
       <c r="B53" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>2005</v>
+        <v>2010</v>
       </c>
       <c r="B54" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C54">
-        <v>3</v>
+        <f>SUM(C53,D54)</f>
+        <v>4</v>
       </c>
       <c r="D54">
         <v>3</v>
       </c>
       <c r="E54" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>2005</v>
+        <v>2010</v>
       </c>
       <c r="B55" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C55">
-        <v>21</v>
+        <f>SUM(C54,D55)</f>
+        <v>31</v>
       </c>
       <c r="D55">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E55" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>2004</v>
+        <v>2011</v>
       </c>
       <c r="B56" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E56" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>2004</v>
+        <v>2011</v>
       </c>
       <c r="B57" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C57">
-        <v>5</v>
+        <f>SUM(C56,D57)</f>
+        <v>7</v>
       </c>
       <c r="D57">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E57" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>2004</v>
+        <v>2011</v>
       </c>
       <c r="B58" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C58">
-        <v>17</v>
+        <f>SUM(C57,D58)</f>
+        <v>51</v>
       </c>
       <c r="D58">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="E58" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>2003</v>
+        <v>2012</v>
       </c>
       <c r="B59" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>2003</v>
+        <v>2012</v>
       </c>
       <c r="B60" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C60">
-        <v>4</v>
+        <f>SUM(C59,D60)</f>
+        <v>11</v>
       </c>
       <c r="D60">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E60" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>2003</v>
+        <v>2012</v>
       </c>
       <c r="B61" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C61">
-        <v>20</v>
+        <f>SUM(C60,D61)</f>
+        <v>39</v>
       </c>
       <c r="D61">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E61" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>2002</v>
+        <v>2013</v>
       </c>
       <c r="B62" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E62" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>2002</v>
+        <v>2013</v>
       </c>
       <c r="B63" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C63">
-        <v>2</v>
+        <f>SUM(C62,D63)</f>
+        <v>5</v>
       </c>
       <c r="D63">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E63" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>2002</v>
+        <v>2013</v>
       </c>
       <c r="B64" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C64">
-        <v>11</v>
+        <f>SUM(C63,D64)</f>
+        <v>46</v>
       </c>
       <c r="D64">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="E64" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>2001</v>
+        <v>2014</v>
       </c>
       <c r="B65" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -1524,452 +1569,475 @@
         <v>0</v>
       </c>
       <c r="E65" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>2001</v>
+        <v>2014</v>
       </c>
       <c r="B66" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C66">
-        <v>2</v>
+        <f>SUM(C65,D66)</f>
+        <v>15</v>
       </c>
       <c r="D66">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E66" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>2001</v>
+        <v>2014</v>
       </c>
       <c r="B67" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C67">
-        <v>15</v>
+        <f>SUM(C66,D67)</f>
+        <v>60</v>
       </c>
       <c r="D67">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="E67" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>2000</v>
+        <v>2015</v>
       </c>
       <c r="B68" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D68">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E68" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>2000</v>
+        <v>2015</v>
       </c>
       <c r="B69" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C69">
-        <v>3</v>
+        <f>SUM(C68,D69)</f>
+        <v>16</v>
       </c>
       <c r="D69">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E69" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>2000</v>
+        <v>2015</v>
       </c>
       <c r="B70" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C70">
-        <v>7</v>
+        <f>SUM(C69,D70)</f>
+        <v>57</v>
       </c>
       <c r="D70">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="E70" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>1999</v>
+        <v>2016</v>
       </c>
       <c r="B71" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>1999</v>
+        <v>2016</v>
       </c>
       <c r="B72" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C72">
-        <v>2</v>
+        <f>SUM(C71,D72)</f>
+        <v>14</v>
       </c>
       <c r="D72">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E72" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>1999</v>
+        <v>2016</v>
       </c>
       <c r="B73" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C73">
-        <v>14</v>
+        <f>SUM(C72,D73)</f>
+        <v>54</v>
       </c>
       <c r="D73">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="E73" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>1998</v>
+        <v>2017</v>
       </c>
       <c r="B74" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C74">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D74">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E74" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>1998</v>
+        <v>2017</v>
       </c>
       <c r="B75" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C75">
-        <v>2</v>
+        <f>SUM(C74,D75)</f>
+        <v>12</v>
       </c>
       <c r="D75">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E75" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>1998</v>
+        <v>2017</v>
       </c>
       <c r="B76" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C76">
-        <v>8</v>
+        <f>SUM(C75,D76)</f>
+        <v>58</v>
       </c>
       <c r="D76">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="E76" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>1997</v>
+        <v>2018</v>
       </c>
       <c r="B77" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E77" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>1997</v>
+        <v>2018</v>
       </c>
       <c r="B78" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C78">
-        <v>2</v>
+        <f>SUM(C77,D78)</f>
+        <v>17</v>
       </c>
       <c r="D78">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E78" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>1997</v>
+        <v>2018</v>
       </c>
       <c r="B79" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C79">
-        <v>13</v>
+        <f>SUM(C78,D79)</f>
+        <v>54</v>
       </c>
       <c r="D79">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="E79" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>1996</v>
+        <v>2019</v>
       </c>
       <c r="B80" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>1996</v>
+        <v>2019</v>
       </c>
       <c r="B81" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C81">
-        <v>2</v>
+        <f>SUM(C80,D81)</f>
+        <v>17</v>
       </c>
       <c r="D81">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E81" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>1996</v>
+        <v>2019</v>
       </c>
       <c r="B82" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C82">
-        <v>8</v>
+        <f>SUM(C81,D82)</f>
+        <v>56</v>
       </c>
       <c r="D82">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="E82" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>1995</v>
+        <v>2020</v>
       </c>
       <c r="B83" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D83">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E83" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>1995</v>
+        <v>2020</v>
       </c>
       <c r="B84" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C84">
-        <v>2</v>
+        <f>SUM(C83,D84)</f>
+        <v>26</v>
       </c>
       <c r="D84">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E84" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>1995</v>
+        <v>2020</v>
       </c>
       <c r="B85" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C85">
-        <v>8</v>
+        <f>SUM(C84,D85)</f>
+        <v>63</v>
       </c>
       <c r="D85">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="E85" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>1994</v>
+        <v>2021</v>
       </c>
       <c r="B86" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C86">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D86">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E86" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>1994</v>
+        <v>2021</v>
       </c>
       <c r="B87" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C87">
-        <v>1</v>
+        <f>SUM(C86,D87)</f>
+        <v>22</v>
       </c>
       <c r="D87">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E87" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>1994</v>
+        <v>2021</v>
       </c>
       <c r="B88" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C88">
-        <v>4</v>
+        <f>SUM(C87,D88)</f>
+        <v>52</v>
       </c>
       <c r="D88">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="E88" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>1993</v>
+        <v>2022</v>
       </c>
       <c r="B89" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D89">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E89" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90">
-        <v>1993</v>
+        <v>2022</v>
       </c>
       <c r="B90" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C90">
-        <v>1</v>
+        <f>SUM(C89,D90)</f>
+        <v>14</v>
       </c>
       <c r="D90">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E90" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>1993</v>
+        <v>2022</v>
       </c>
       <c r="B91" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C91">
-        <v>9</v>
+        <f>SUM(C90,D91)</f>
+        <v>59</v>
       </c>
       <c r="D91">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="E91" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E91" xr:uid="{4328A730-E7CA-3945-A5F9-D48A384393CA}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E91">
+      <sortCondition ref="A1:A91"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>